<commit_message>
Mejoras y correcciones en el API
</commit_message>
<xml_diff>
--- a/Reporte/ReportesSigre.xlsx
+++ b/Reporte/ReportesSigre.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\SigreWeb\sigreweb-main\api-Sigre\Reporte\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\SigreWeb\sigreweb-main\SigreApiRest\Reporte\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D96C625B-2CB4-44D7-8B4E-02AFBE61BA6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45383497-7D6F-46E6-93CD-74FBE695B4AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{4481B342-BB1C-481E-A30A-ED1416DC2C19}"/>
+    <workbookView xWindow="1335" yWindow="750" windowWidth="25695" windowHeight="14055" xr2:uid="{4481B342-BB1C-481E-A30A-ED1416DC2C19}"/>
   </bookViews>
   <sheets>
     <sheet name="BT" sheetId="1" r:id="rId1"/>
@@ -26,15 +26,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="38">
   <si>
     <t xml:space="preserve">NOMBRE RESP:      </t>
   </si>
   <si>
     <t>FECHA:</t>
-  </si>
-  <si>
-    <t>Etiqueta</t>
   </si>
   <si>
     <t>-</t>
@@ -50,9 +47,6 @@
  MINIMAS DE SEGURIDAD</t>
   </si>
   <si>
-    <t>RESULTADO</t>
-  </si>
-  <si>
     <t>Codigo Deficiencia</t>
   </si>
   <si>
@@ -128,9 +122,6 @@
     <t xml:space="preserve">SED: </t>
   </si>
   <si>
-    <t>PAG N°:</t>
-  </si>
-  <si>
     <t>CÓDIGOS</t>
   </si>
   <si>
@@ -147,13 +138,19 @@
   </si>
   <si>
     <t>DEFICIENCIAS EN REDES DE BAJA TENSION</t>
+  </si>
+  <si>
+    <t>Circuito</t>
+  </si>
+  <si>
+    <t>ORDEN N°:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -210,11 +207,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b/>
       <sz val="16"/>
       <color theme="1"/>
@@ -262,6 +254,31 @@
       <b/>
       <sz val="8"/>
       <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -328,7 +345,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="55">
+  <borders count="54">
     <border>
       <left/>
       <right/>
@@ -712,21 +729,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="medium">
         <color indexed="64"/>
@@ -893,36 +895,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -1024,14 +996,38 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="155">
+  <cellXfs count="160">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1058,9 +1054,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1087,16 +1080,10 @@
     </xf>
     <xf numFmtId="49" fontId="3" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1105,12 +1092,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1129,25 +1110,19 @@
     <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="14" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="14" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="3" fillId="9" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
@@ -1160,7 +1135,7 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="10" fillId="10" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="9" fillId="10" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="7" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1184,7 +1159,7 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1193,10 +1168,10 @@
     <xf numFmtId="0" fontId="8" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="3" fillId="9" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="9" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="3" fillId="9" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="9" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="20" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1208,31 +1183,19 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="6" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="13" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="13" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="38" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="37" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1253,18 +1216,6 @@
     <xf numFmtId="49" fontId="3" fillId="5" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
@@ -1301,19 +1252,19 @@
     <xf numFmtId="49" fontId="3" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="5" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="34" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="5" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="33" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="40" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="39" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="19" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1325,53 +1276,47 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="41" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="40" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="21" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="9" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="51" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="9" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="48" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="3" fillId="2" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="10" fillId="10" borderId="53" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="54" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="3" fillId="2" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="9" fillId="10" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="51" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1383,19 +1328,74 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="4" borderId="12" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="4" borderId="22" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="4" borderId="25" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="3" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1407,25 +1407,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -1455,19 +1455,28 @@
     <xf numFmtId="1" fontId="3" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1476,7 +1485,17 @@
     <cellStyle name="Normal 2" xfId="2" xr:uid="{12DC15DF-CA1F-4245-9A2D-A5E057ADE674}"/>
     <cellStyle name="Normal 3" xfId="3" xr:uid="{4FB8B8F2-A749-4C66-B66E-3C2638139B5D}"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1797,22 +1816,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2753035-815A-40F2-8A73-CB51F15BF724}">
-  <dimension ref="A1:O42"/>
+  <dimension ref="A1:V42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="12" topLeftCell="M1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="I1" sqref="I1"/>
+      <selection pane="topRight" activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.7109375" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="3.85546875" hidden="1" customWidth="1"/>
-    <col min="3" max="5" width="5.85546875" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="4.42578125" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="1.85546875" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="2.85546875" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="3.7109375" customWidth="1"/>
+    <col min="1" max="1" width="1.7109375" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="2.28515625" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="2.85546875" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="1.5703125" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="2" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="1.28515625" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="2" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="1.7109375" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="2.28515625" hidden="1" customWidth="1"/>
     <col min="10" max="10" width="4.85546875" customWidth="1"/>
     <col min="11" max="11" width="8" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="76.140625" bestFit="1" customWidth="1"/>
@@ -1820,396 +1841,386 @@
     <col min="14" max="15" width="19.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="43"/>
-    </row>
-    <row r="2" spans="1:15" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="36"/>
+    </row>
+    <row r="2" spans="1:22" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K2" s="1"/>
       <c r="L2" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="M2" s="3"/>
-      <c r="N2" s="136" t="s">
-        <v>14</v>
-      </c>
-      <c r="O2" s="137"/>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N2" s="138" t="s">
+        <v>12</v>
+      </c>
+      <c r="O2" s="139"/>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="K3" s="4"/>
       <c r="L3" s="5"/>
       <c r="M3" s="6"/>
-      <c r="N3" s="140"/>
-      <c r="O3" s="141"/>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N3" s="142"/>
+      <c r="O3" s="143"/>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="K4" s="4"/>
       <c r="L4" s="7"/>
       <c r="M4" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="N4" s="142"/>
-      <c r="O4" s="143"/>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N4" s="144"/>
+      <c r="O4" s="145"/>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="K5" s="4"/>
       <c r="L5" s="9"/>
       <c r="M5" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="N5" s="142"/>
-      <c r="O5" s="143"/>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="N5" s="144"/>
+      <c r="O5" s="145"/>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="K6" s="4"/>
       <c r="L6" s="9"/>
       <c r="M6" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="N6" s="138"/>
-      <c r="O6" s="139"/>
-    </row>
-    <row r="7" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N6" s="140"/>
+      <c r="O6" s="141"/>
+    </row>
+    <row r="7" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K7" s="10"/>
       <c r="L7" s="11"/>
-      <c r="M7" s="73" t="s">
+      <c r="M7" s="62" t="s">
+        <v>37</v>
+      </c>
+      <c r="N7" s="9"/>
+      <c r="O7" s="60"/>
+    </row>
+    <row r="8" spans="1:22" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="13"/>
+      <c r="B8" s="126" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="129" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="135" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="132" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" s="37"/>
+      <c r="H8" s="37"/>
+      <c r="K8" s="111"/>
+      <c r="L8" s="109" t="s">
+        <v>31</v>
+      </c>
+      <c r="M8" s="13"/>
+      <c r="N8" s="123"/>
+      <c r="O8" s="124"/>
+    </row>
+    <row r="9" spans="1:22" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="14"/>
+      <c r="B9" s="127"/>
+      <c r="C9" s="130"/>
+      <c r="D9" s="136"/>
+      <c r="E9" s="133"/>
+      <c r="G9" s="37"/>
+      <c r="H9" s="37"/>
+      <c r="K9" s="56"/>
+      <c r="L9" s="91" t="s">
+        <v>28</v>
+      </c>
+      <c r="M9" s="120"/>
+      <c r="N9" s="121"/>
+      <c r="O9" s="122"/>
+      <c r="V9" s="37"/>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A10" s="15"/>
+      <c r="B10" s="127"/>
+      <c r="C10" s="130"/>
+      <c r="D10" s="136"/>
+      <c r="E10" s="133"/>
+      <c r="G10" s="37"/>
+      <c r="H10" s="37"/>
+      <c r="K10" s="81"/>
+      <c r="L10" s="61" t="s">
+        <v>17</v>
+      </c>
+      <c r="M10" s="75"/>
+      <c r="N10" s="64"/>
+      <c r="O10" s="69"/>
+      <c r="V10" s="37"/>
+    </row>
+    <row r="11" spans="1:22" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="16"/>
+      <c r="B11" s="127"/>
+      <c r="C11" s="131"/>
+      <c r="D11" s="136"/>
+      <c r="E11" s="133"/>
+      <c r="G11" s="37"/>
+      <c r="H11" s="37"/>
+      <c r="K11" s="84">
+        <v>6002</v>
+      </c>
+      <c r="L11" s="54" t="s">
+        <v>18</v>
+      </c>
+      <c r="M11" s="75"/>
+      <c r="N11" s="64"/>
+      <c r="O11" s="69"/>
+      <c r="V11" s="37"/>
+    </row>
+    <row r="12" spans="1:22" ht="55.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="16"/>
+      <c r="B12" s="128"/>
+      <c r="C12" s="44">
+        <v>0</v>
+      </c>
+      <c r="D12" s="137"/>
+      <c r="E12" s="134"/>
+      <c r="G12" s="37"/>
+      <c r="H12" s="37"/>
+      <c r="K12" s="84">
+        <v>6004</v>
+      </c>
+      <c r="L12" s="54" t="s">
+        <v>19</v>
+      </c>
+      <c r="M12" s="75"/>
+      <c r="N12" s="64"/>
+      <c r="O12" s="69"/>
+      <c r="V12" s="37"/>
+    </row>
+    <row r="13" spans="1:22" ht="63" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="16"/>
+      <c r="B13" s="33">
+        <v>6002</v>
+      </c>
+      <c r="C13" s="43"/>
+      <c r="D13" s="35"/>
+      <c r="E13" s="39"/>
+      <c r="G13" s="38"/>
+      <c r="H13" s="38"/>
+      <c r="K13" s="85">
+        <v>6006</v>
+      </c>
+      <c r="L13" s="54" t="s">
+        <v>20</v>
+      </c>
+      <c r="M13" s="75"/>
+      <c r="N13" s="64"/>
+      <c r="O13" s="69"/>
+      <c r="V13" s="37"/>
+    </row>
+    <row r="14" spans="1:22" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="17"/>
+      <c r="B14" s="26">
+        <v>6004</v>
+      </c>
+      <c r="C14" s="27"/>
+      <c r="D14" s="28"/>
+      <c r="E14" s="40"/>
+      <c r="G14" s="38"/>
+      <c r="H14" s="38"/>
+      <c r="K14" s="86">
+        <v>6008</v>
+      </c>
+      <c r="L14" s="82" t="s">
+        <v>21</v>
+      </c>
+      <c r="M14" s="76"/>
+      <c r="N14" s="65"/>
+      <c r="O14" s="70"/>
+      <c r="V14" s="38"/>
+    </row>
+    <row r="15" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="18"/>
+      <c r="B15" s="26">
+        <v>6006</v>
+      </c>
+      <c r="C15" s="27"/>
+      <c r="D15" s="28"/>
+      <c r="E15" s="40"/>
+      <c r="G15" s="38"/>
+      <c r="H15" s="38"/>
+      <c r="K15" s="55"/>
+      <c r="L15" s="91" t="s">
+        <v>14</v>
+      </c>
+      <c r="M15" s="77"/>
+      <c r="N15" s="63"/>
+      <c r="O15" s="68"/>
+      <c r="V15" s="38"/>
+    </row>
+    <row r="16" spans="1:22" ht="42.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="18"/>
+      <c r="B16" s="26">
+        <v>6008</v>
+      </c>
+      <c r="C16" s="27"/>
+      <c r="D16" s="28"/>
+      <c r="E16" s="40"/>
+      <c r="G16" s="38"/>
+      <c r="H16" s="38"/>
+      <c r="K16" s="86">
+        <v>6024</v>
+      </c>
+      <c r="L16" s="61" t="s">
+        <v>22</v>
+      </c>
+      <c r="M16" s="75"/>
+      <c r="N16" s="64"/>
+      <c r="O16" s="69"/>
+      <c r="V16" s="38"/>
+    </row>
+    <row r="17" spans="1:22" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="18"/>
+      <c r="B17" s="26">
+        <v>6024</v>
+      </c>
+      <c r="C17" s="27"/>
+      <c r="D17" s="28"/>
+      <c r="E17" s="40"/>
+      <c r="G17" s="38"/>
+      <c r="H17" s="38"/>
+      <c r="K17" s="89"/>
+      <c r="L17" s="61" t="s">
+        <v>23</v>
+      </c>
+      <c r="M17" s="78"/>
+      <c r="N17" s="66"/>
+      <c r="O17" s="71"/>
+      <c r="V17" s="38"/>
+    </row>
+    <row r="18" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="17"/>
+      <c r="B18" s="26">
+        <v>6026</v>
+      </c>
+      <c r="C18" s="27"/>
+      <c r="D18" s="28"/>
+      <c r="E18" s="40"/>
+      <c r="K18" s="55"/>
+      <c r="L18" s="91" t="s">
+        <v>11</v>
+      </c>
+      <c r="M18" s="77"/>
+      <c r="N18" s="63"/>
+      <c r="O18" s="68"/>
+      <c r="V18" s="38"/>
+    </row>
+    <row r="19" spans="1:22" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="B19" s="26">
+        <v>6028</v>
+      </c>
+      <c r="C19" s="27"/>
+      <c r="D19" s="28"/>
+      <c r="E19" s="40"/>
+      <c r="K19" s="90">
+        <v>6026</v>
+      </c>
+      <c r="L19" s="61" t="s">
+        <v>15</v>
+      </c>
+      <c r="M19" s="75"/>
+      <c r="N19" s="64"/>
+      <c r="O19" s="69"/>
+    </row>
+    <row r="20" spans="1:22" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="B20" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" s="30"/>
+      <c r="D20" s="41"/>
+      <c r="E20" s="42"/>
+      <c r="K20" s="86">
+        <v>6028</v>
+      </c>
+      <c r="L20" s="94" t="s">
+        <v>16</v>
+      </c>
+      <c r="M20" s="75"/>
+      <c r="N20" s="64"/>
+      <c r="O20" s="69"/>
+    </row>
+    <row r="21" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="17"/>
+      <c r="K21" s="55"/>
+      <c r="L21" s="91"/>
+      <c r="M21" s="77"/>
+      <c r="N21" s="63"/>
+      <c r="O21" s="68"/>
+    </row>
+    <row r="22" spans="1:22" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="K22" s="93"/>
+      <c r="L22" s="115" t="s">
+        <v>36</v>
+      </c>
+      <c r="M22" s="112"/>
+      <c r="N22" s="113"/>
+      <c r="O22" s="114"/>
+    </row>
+    <row r="23" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="20"/>
+      <c r="K23" s="4"/>
+      <c r="L23" s="106" t="s">
         <v>32</v>
       </c>
-      <c r="N7" s="70"/>
-      <c r="O7" s="71"/>
-    </row>
-    <row r="8" spans="1:15" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="B8" s="124" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="127" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" s="133" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" s="130" t="s">
-        <v>12</v>
-      </c>
-      <c r="F8" s="44"/>
-      <c r="G8" s="44"/>
-      <c r="H8" s="44"/>
-      <c r="K8" s="104" t="s">
-        <v>33</v>
-      </c>
-      <c r="L8" s="109" t="s">
-        <v>34</v>
-      </c>
-      <c r="M8" s="79"/>
-      <c r="N8" s="80"/>
-      <c r="O8" s="81"/>
-    </row>
-    <row r="9" spans="1:15" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="15"/>
-      <c r="B9" s="125"/>
-      <c r="C9" s="128"/>
-      <c r="D9" s="134"/>
-      <c r="E9" s="131"/>
-      <c r="F9" s="44"/>
-      <c r="G9" s="44"/>
-      <c r="H9" s="44"/>
-      <c r="K9" s="63"/>
-      <c r="L9" s="107" t="s">
-        <v>30</v>
-      </c>
-      <c r="M9" s="82"/>
-      <c r="N9" s="74"/>
-      <c r="O9" s="83"/>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="16"/>
-      <c r="B10" s="125"/>
-      <c r="C10" s="128"/>
-      <c r="D10" s="134"/>
-      <c r="E10" s="131"/>
-      <c r="F10" s="44"/>
-      <c r="G10" s="44"/>
-      <c r="H10" s="44"/>
-      <c r="K10" s="96"/>
-      <c r="L10" s="72" t="s">
-        <v>19</v>
-      </c>
-      <c r="M10" s="90"/>
-      <c r="N10" s="75"/>
-      <c r="O10" s="84"/>
-    </row>
-    <row r="11" spans="1:15" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="17"/>
-      <c r="B11" s="125"/>
-      <c r="C11" s="129"/>
-      <c r="D11" s="134"/>
-      <c r="E11" s="131"/>
-      <c r="F11" s="44"/>
-      <c r="G11" s="44"/>
-      <c r="H11" s="44"/>
-      <c r="K11" s="99">
-        <v>6002</v>
-      </c>
-      <c r="L11" s="61" t="s">
-        <v>20</v>
-      </c>
-      <c r="M11" s="90"/>
-      <c r="N11" s="75"/>
-      <c r="O11" s="84"/>
-    </row>
-    <row r="12" spans="1:15" ht="55.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="17"/>
-      <c r="B12" s="126"/>
-      <c r="C12" s="51">
+      <c r="M23" s="79"/>
+      <c r="N23" s="67"/>
+      <c r="O23" s="72"/>
+    </row>
+    <row r="24" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="32"/>
+      <c r="K24" s="92"/>
+      <c r="L24" s="83" t="s">
+        <v>3</v>
+      </c>
+      <c r="M24" s="80"/>
+      <c r="N24" s="73"/>
+      <c r="O24" s="74"/>
+    </row>
+    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A28" s="25">
         <v>0</v>
       </c>
-      <c r="D12" s="135"/>
-      <c r="E12" s="132"/>
-      <c r="F12" s="44"/>
-      <c r="G12" s="44"/>
-      <c r="H12" s="44"/>
-      <c r="K12" s="99">
-        <v>6004</v>
-      </c>
-      <c r="L12" s="61" t="s">
-        <v>21</v>
-      </c>
-      <c r="M12" s="90"/>
-      <c r="N12" s="75"/>
-      <c r="O12" s="84"/>
-    </row>
-    <row r="13" spans="1:15" ht="63" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="17"/>
-      <c r="B13" s="40">
-        <v>6002</v>
-      </c>
-      <c r="C13" s="50"/>
-      <c r="D13" s="42"/>
-      <c r="E13" s="46"/>
-      <c r="F13" s="45"/>
-      <c r="G13" s="45"/>
-      <c r="H13" s="45"/>
-      <c r="K13" s="100">
-        <v>6006</v>
-      </c>
-      <c r="L13" s="61" t="s">
-        <v>22</v>
-      </c>
-      <c r="M13" s="90"/>
-      <c r="N13" s="75"/>
-      <c r="O13" s="84"/>
-    </row>
-    <row r="14" spans="1:15" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="18"/>
-      <c r="B14" s="31">
-        <v>6004</v>
-      </c>
-      <c r="C14" s="32"/>
-      <c r="D14" s="33"/>
-      <c r="E14" s="47"/>
-      <c r="F14" s="45"/>
-      <c r="G14" s="45"/>
-      <c r="H14" s="45"/>
-      <c r="K14" s="101">
-        <v>6008</v>
-      </c>
-      <c r="L14" s="97" t="s">
-        <v>23</v>
-      </c>
-      <c r="M14" s="91"/>
-      <c r="N14" s="76"/>
-      <c r="O14" s="85"/>
-    </row>
-    <row r="15" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="19"/>
-      <c r="B15" s="31">
-        <v>6006</v>
-      </c>
-      <c r="C15" s="32"/>
-      <c r="D15" s="33"/>
-      <c r="E15" s="47"/>
-      <c r="F15" s="45"/>
-      <c r="G15" s="45"/>
-      <c r="H15" s="45"/>
-      <c r="K15" s="62"/>
-      <c r="L15" s="107" t="s">
-        <v>16</v>
-      </c>
-      <c r="M15" s="92"/>
-      <c r="N15" s="74"/>
-      <c r="O15" s="83"/>
-    </row>
-    <row r="16" spans="1:15" ht="42.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="19"/>
-      <c r="B16" s="31">
-        <v>6008</v>
-      </c>
-      <c r="C16" s="32"/>
-      <c r="D16" s="33"/>
-      <c r="E16" s="47"/>
-      <c r="F16" s="45"/>
-      <c r="G16" s="45"/>
-      <c r="H16" s="45"/>
-      <c r="K16" s="101">
-        <v>6024</v>
-      </c>
-      <c r="L16" s="72" t="s">
-        <v>24</v>
-      </c>
-      <c r="M16" s="90"/>
-      <c r="N16" s="75"/>
-      <c r="O16" s="84"/>
-    </row>
-    <row r="17" spans="1:15" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="19"/>
-      <c r="B17" s="31">
-        <v>6024</v>
-      </c>
-      <c r="C17" s="32"/>
-      <c r="D17" s="33"/>
-      <c r="E17" s="47"/>
-      <c r="F17" s="45"/>
-      <c r="G17" s="45"/>
-      <c r="H17" s="45"/>
-      <c r="K17" s="105"/>
-      <c r="L17" s="72" t="s">
-        <v>25</v>
-      </c>
-      <c r="M17" s="93"/>
-      <c r="N17" s="77"/>
-      <c r="O17" s="86"/>
-    </row>
-    <row r="18" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="18"/>
-      <c r="B18" s="31">
-        <v>6026</v>
-      </c>
-      <c r="C18" s="32"/>
-      <c r="D18" s="33"/>
-      <c r="E18" s="47"/>
-      <c r="K18" s="62"/>
-      <c r="L18" s="107" t="s">
-        <v>13</v>
-      </c>
-      <c r="M18" s="92"/>
-      <c r="N18" s="74"/>
-      <c r="O18" s="83"/>
-    </row>
-    <row r="19" spans="1:15" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="20" t="s">
-        <v>3</v>
-      </c>
-      <c r="B19" s="31">
-        <v>6028</v>
-      </c>
-      <c r="C19" s="32"/>
-      <c r="D19" s="33"/>
-      <c r="E19" s="47"/>
-      <c r="K19" s="106">
-        <v>6026</v>
-      </c>
-      <c r="L19" s="72" t="s">
-        <v>17</v>
-      </c>
-      <c r="M19" s="90"/>
-      <c r="N19" s="75"/>
-      <c r="O19" s="84"/>
-    </row>
-    <row r="20" spans="1:15" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="20" t="s">
-        <v>3</v>
-      </c>
-      <c r="B20" s="34" t="s">
-        <v>11</v>
-      </c>
-      <c r="C20" s="35"/>
-      <c r="D20" s="48"/>
-      <c r="E20" s="49"/>
-      <c r="K20" s="101">
-        <v>6028</v>
-      </c>
-      <c r="L20" s="111" t="s">
-        <v>18</v>
-      </c>
-      <c r="M20" s="90"/>
-      <c r="N20" s="75"/>
-      <c r="O20" s="84"/>
-    </row>
-    <row r="21" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="18"/>
-      <c r="K21" s="62"/>
-      <c r="L21" s="107"/>
-      <c r="M21" s="92"/>
-      <c r="N21" s="74"/>
-      <c r="O21" s="83"/>
-    </row>
-    <row r="22" spans="1:15" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="K22" s="110"/>
-      <c r="L22" s="98"/>
-      <c r="M22" s="93"/>
-      <c r="N22" s="77"/>
-      <c r="O22" s="86"/>
-    </row>
-    <row r="23" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="21"/>
-      <c r="K23" s="4"/>
-      <c r="L23" s="123" t="s">
-        <v>35</v>
-      </c>
-      <c r="M23" s="94"/>
-      <c r="N23" s="78"/>
-      <c r="O23" s="87"/>
-    </row>
-    <row r="24" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="39"/>
-      <c r="K24" s="108"/>
-      <c r="L24" s="98" t="s">
-        <v>4</v>
-      </c>
-      <c r="M24" s="95"/>
-      <c r="N24" s="88"/>
-      <c r="O24" s="89"/>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A28" s="28">
-        <v>0</v>
-      </c>
-      <c r="L28" s="29">
-        <v>0</v>
-      </c>
-      <c r="M28" s="28"/>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A29" s="28"/>
-      <c r="L29" s="30" t="s">
-        <v>7</v>
-      </c>
-      <c r="M29" s="28"/>
+    </row>
+    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A29" s="25"/>
     </row>
     <row r="33" spans="3:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="35" spans="3:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="38" spans="3:9" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="39" spans="3:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="41" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="E41" s="27"/>
-      <c r="F41" s="27"/>
-      <c r="G41" s="27"/>
-      <c r="H41" s="27"/>
-      <c r="I41" s="27"/>
+      <c r="E41" s="24"/>
+      <c r="F41" s="24"/>
+      <c r="G41" s="24"/>
+      <c r="H41" s="24"/>
+      <c r="I41" s="24"/>
     </row>
     <row r="42" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C42" s="36"/>
-      <c r="D42" s="36"/>
-      <c r="E42" s="27"/>
-      <c r="F42" s="27"/>
-      <c r="G42" s="27"/>
-      <c r="H42" s="27"/>
-      <c r="I42" s="27"/>
+      <c r="C42" s="31"/>
+      <c r="D42" s="31"/>
+      <c r="E42" s="24"/>
+      <c r="F42" s="24"/>
+      <c r="G42" s="24"/>
+      <c r="H42" s="24"/>
+      <c r="I42" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -2223,8 +2234,8 @@
     <mergeCell ref="N4:O4"/>
     <mergeCell ref="N5:O5"/>
   </mergeCells>
-  <conditionalFormatting sqref="K8:L8">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  <conditionalFormatting sqref="L8">
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2237,20 +2248,22 @@
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="12" topLeftCell="M1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="P25" sqref="P25"/>
+      <selection pane="topRight" activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="0.28515625" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="38.5703125" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="25.85546875" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="69.5703125" hidden="1" customWidth="1"/>
-    <col min="6" max="8" width="13" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="4.140625" customWidth="1"/>
+    <col min="1" max="1" width="2.5703125" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="2.7109375" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="2.28515625" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="3.5703125" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="6.42578125" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="6.85546875" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="5.7109375" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="5.85546875" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="4.140625" hidden="1" customWidth="1"/>
     <col min="10" max="10" width="4.85546875" customWidth="1"/>
-    <col min="11" max="11" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.7109375" customWidth="1"/>
     <col min="12" max="12" width="80.140625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="21.28515625" bestFit="1" customWidth="1"/>
     <col min="14" max="15" width="19.7109375" customWidth="1"/>
@@ -2260,20 +2273,20 @@
     <row r="2" spans="1:15" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K2" s="1"/>
       <c r="L2" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="M2" s="3"/>
-      <c r="N2" s="144" t="s">
-        <v>5</v>
-      </c>
-      <c r="O2" s="145"/>
+      <c r="N2" s="146" t="s">
+        <v>4</v>
+      </c>
+      <c r="O2" s="147"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="K3" s="4"/>
       <c r="L3" s="5"/>
       <c r="M3" s="6"/>
-      <c r="N3" s="140"/>
-      <c r="O3" s="141"/>
+      <c r="N3" s="142"/>
+      <c r="O3" s="143"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="K4" s="4"/>
@@ -2281,254 +2294,250 @@
       <c r="M4" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="N4" s="142"/>
-      <c r="O4" s="143"/>
+      <c r="N4" s="144"/>
+      <c r="O4" s="145"/>
     </row>
     <row r="5" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K5" s="4"/>
       <c r="L5" s="9"/>
       <c r="M5" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="N5" s="142"/>
-      <c r="O5" s="143"/>
+        <v>29</v>
+      </c>
+      <c r="N5" s="144"/>
+      <c r="O5" s="145"/>
     </row>
     <row r="6" spans="1:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="146" t="s">
+      <c r="B6" s="148" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="151" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="154" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="149" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="152" t="s">
+      <c r="E6" s="156" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="154" t="s">
-        <v>12</v>
-      </c>
-      <c r="F6" s="44"/>
-      <c r="G6" s="44"/>
-      <c r="H6" s="44"/>
-      <c r="I6" s="44"/>
+      <c r="F6" s="37"/>
+      <c r="G6" s="37"/>
+      <c r="H6" s="37"/>
+      <c r="I6" s="37"/>
       <c r="K6" s="4"/>
       <c r="L6" s="9"/>
       <c r="M6" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="N6" s="138"/>
-      <c r="O6" s="139"/>
+      <c r="N6" s="140"/>
+      <c r="O6" s="141"/>
     </row>
     <row r="7" spans="1:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="147"/>
-      <c r="C7" s="150"/>
-      <c r="D7" s="147"/>
-      <c r="E7" s="147"/>
-      <c r="I7" s="44"/>
+      <c r="B7" s="149"/>
+      <c r="C7" s="152"/>
+      <c r="D7" s="149"/>
+      <c r="E7" s="149"/>
+      <c r="I7" s="37"/>
       <c r="K7" s="10"/>
       <c r="L7" s="11"/>
-      <c r="M7" s="73" t="s">
+      <c r="M7" s="62" t="s">
+        <v>37</v>
+      </c>
+      <c r="N7" s="159"/>
+      <c r="O7" s="12"/>
+    </row>
+    <row r="8" spans="1:15" ht="18.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="149"/>
+      <c r="C8" s="152"/>
+      <c r="D8" s="149"/>
+      <c r="E8" s="149"/>
+      <c r="I8" s="37"/>
+      <c r="K8" s="116"/>
+      <c r="L8" s="110"/>
+      <c r="M8" s="23"/>
+      <c r="N8" s="23"/>
+      <c r="O8" s="23"/>
+    </row>
+    <row r="9" spans="1:15" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="45"/>
+      <c r="B9" s="149"/>
+      <c r="C9" s="152"/>
+      <c r="D9" s="149"/>
+      <c r="E9" s="149"/>
+      <c r="I9" s="37"/>
+      <c r="K9" s="157" t="s">
+        <v>30</v>
+      </c>
+      <c r="L9" s="118" t="s">
+        <v>33</v>
+      </c>
+      <c r="M9" s="21"/>
+      <c r="N9" s="21"/>
+      <c r="O9" s="21"/>
+    </row>
+    <row r="10" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="46"/>
+      <c r="B10" s="149"/>
+      <c r="C10" s="153"/>
+      <c r="D10" s="149"/>
+      <c r="E10" s="149"/>
+      <c r="I10" s="37"/>
+      <c r="K10" s="158"/>
+      <c r="L10" s="117" t="s">
+        <v>34</v>
+      </c>
+      <c r="M10" s="22"/>
+      <c r="N10" s="22"/>
+      <c r="O10" s="22"/>
+    </row>
+    <row r="11" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="47"/>
+      <c r="B11" s="150"/>
+      <c r="C11" s="51">
+        <v>0</v>
+      </c>
+      <c r="D11" s="155"/>
+      <c r="E11" s="155"/>
+      <c r="I11" s="37"/>
+      <c r="K11" s="91"/>
+      <c r="L11" s="91" t="s">
+        <v>13</v>
+      </c>
+      <c r="M11" s="91"/>
+      <c r="N11" s="91"/>
+      <c r="O11" s="91"/>
+    </row>
+    <row r="12" spans="1:15" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="48"/>
+      <c r="B12" s="102">
+        <v>7002</v>
+      </c>
+      <c r="C12" s="43"/>
+      <c r="D12" s="52"/>
+      <c r="E12" s="39"/>
+      <c r="F12" s="38"/>
+      <c r="G12" s="38"/>
+      <c r="H12" s="38"/>
+      <c r="I12" s="37"/>
+      <c r="K12" s="102">
+        <v>7002</v>
+      </c>
+      <c r="L12" s="58" t="s">
+        <v>24</v>
+      </c>
+      <c r="M12" s="23"/>
+      <c r="N12" s="23"/>
+      <c r="O12" s="23"/>
+    </row>
+    <row r="13" spans="1:15" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="107"/>
+      <c r="B13" s="103">
+        <v>7004</v>
+      </c>
+      <c r="C13" s="27"/>
+      <c r="D13" s="53"/>
+      <c r="E13" s="40"/>
+      <c r="F13" s="38"/>
+      <c r="G13" s="38"/>
+      <c r="H13" s="38"/>
+      <c r="I13" s="38"/>
+      <c r="K13" s="103">
+        <v>7004</v>
+      </c>
+      <c r="L13" s="87" t="s">
+        <v>25</v>
+      </c>
+      <c r="M13" s="108"/>
+      <c r="N13" s="108"/>
+      <c r="O13" s="108"/>
+    </row>
+    <row r="14" spans="1:15" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="48"/>
+      <c r="B14" s="103">
+        <v>7006</v>
+      </c>
+      <c r="C14" s="27"/>
+      <c r="D14" s="53"/>
+      <c r="E14" s="40"/>
+      <c r="F14" s="38"/>
+      <c r="G14" s="38"/>
+      <c r="H14" s="38"/>
+      <c r="I14" s="38"/>
+      <c r="K14" s="103">
+        <v>7006</v>
+      </c>
+      <c r="L14" s="88" t="s">
+        <v>26</v>
+      </c>
+      <c r="M14" s="59"/>
+      <c r="N14" s="59"/>
+      <c r="O14" s="59"/>
+    </row>
+    <row r="15" spans="1:15" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="48"/>
+      <c r="B15" s="104">
+        <v>7008</v>
+      </c>
+      <c r="C15" s="95"/>
+      <c r="D15" s="96"/>
+      <c r="E15" s="97"/>
+      <c r="I15" s="38"/>
+      <c r="K15" s="103">
+        <v>7008</v>
+      </c>
+      <c r="L15" s="88" t="s">
+        <v>27</v>
+      </c>
+      <c r="M15" s="59"/>
+      <c r="N15" s="59"/>
+      <c r="O15" s="59"/>
+    </row>
+    <row r="16" spans="1:15" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="49"/>
+      <c r="B16" s="98" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="99"/>
+      <c r="D16" s="100"/>
+      <c r="E16" s="101"/>
+      <c r="I16" s="38"/>
+      <c r="K16" s="91"/>
+      <c r="L16" s="119" t="s">
+        <v>36</v>
+      </c>
+      <c r="M16" s="125"/>
+      <c r="N16" s="125"/>
+      <c r="O16" s="125"/>
+    </row>
+    <row r="17" spans="1:15" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="105"/>
+      <c r="K17" s="23"/>
+      <c r="L17" s="106" t="s">
         <v>32</v>
       </c>
-      <c r="N7" s="12"/>
-      <c r="O7" s="13"/>
-    </row>
-    <row r="8" spans="1:15" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="147"/>
-      <c r="C8" s="150"/>
-      <c r="D8" s="147"/>
-      <c r="E8" s="147"/>
-      <c r="I8" s="44"/>
-      <c r="K8" s="4"/>
-      <c r="L8" s="65"/>
-      <c r="M8" s="26"/>
-      <c r="N8" s="26"/>
-      <c r="O8" s="26"/>
-    </row>
-    <row r="9" spans="1:15" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="52"/>
-      <c r="B9" s="147"/>
-      <c r="C9" s="150"/>
-      <c r="D9" s="147"/>
-      <c r="E9" s="147"/>
-      <c r="I9" s="44"/>
-      <c r="K9" s="22"/>
-      <c r="L9" s="66" t="s">
-        <v>36</v>
-      </c>
-      <c r="M9" s="23"/>
-      <c r="N9" s="23"/>
-      <c r="O9" s="23"/>
-    </row>
-    <row r="10" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="53"/>
-      <c r="B10" s="147"/>
-      <c r="C10" s="151"/>
-      <c r="D10" s="147"/>
-      <c r="E10" s="147"/>
-      <c r="I10" s="44"/>
-      <c r="K10" s="24"/>
-      <c r="L10" s="67" t="s">
-        <v>37</v>
-      </c>
-      <c r="M10" s="25"/>
-      <c r="N10" s="25"/>
-      <c r="O10" s="25"/>
-    </row>
-    <row r="11" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="54"/>
-      <c r="B11" s="148"/>
-      <c r="C11" s="58">
+      <c r="M17" s="57"/>
+      <c r="N17" s="57"/>
+      <c r="O17" s="57"/>
+    </row>
+    <row r="18" spans="1:15" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="50"/>
+      <c r="K18" s="23"/>
+      <c r="L18" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="M18" s="22"/>
+      <c r="N18" s="22"/>
+      <c r="O18" s="22"/>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A22" s="25">
         <v>0</v>
       </c>
-      <c r="D11" s="153"/>
-      <c r="E11" s="153"/>
-      <c r="I11" s="44"/>
-      <c r="K11" s="107"/>
-      <c r="L11" s="107" t="s">
-        <v>15</v>
-      </c>
-      <c r="M11" s="107"/>
-      <c r="N11" s="107"/>
-      <c r="O11" s="107"/>
-    </row>
-    <row r="12" spans="1:15" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="55"/>
-      <c r="B12" s="119">
-        <v>7002</v>
-      </c>
-      <c r="C12" s="50"/>
-      <c r="D12" s="59"/>
-      <c r="E12" s="46"/>
-      <c r="F12" s="45"/>
-      <c r="G12" s="45"/>
-      <c r="H12" s="45"/>
-      <c r="I12" s="44"/>
-      <c r="K12" s="119">
-        <v>7002</v>
-      </c>
-      <c r="L12" s="68" t="s">
-        <v>26</v>
-      </c>
-      <c r="M12" s="26"/>
-      <c r="N12" s="26"/>
-      <c r="O12" s="26"/>
-    </row>
-    <row r="13" spans="1:15" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="55"/>
-      <c r="B13" s="120">
-        <v>7004</v>
-      </c>
-      <c r="C13" s="32"/>
-      <c r="D13" s="60"/>
-      <c r="E13" s="47"/>
-      <c r="F13" s="45"/>
-      <c r="G13" s="45"/>
-      <c r="H13" s="45"/>
-      <c r="I13" s="45"/>
-      <c r="K13" s="120">
-        <v>7004</v>
-      </c>
-      <c r="L13" s="102" t="s">
-        <v>27</v>
-      </c>
-      <c r="M13" s="26"/>
-      <c r="N13" s="26"/>
-      <c r="O13" s="26"/>
-    </row>
-    <row r="14" spans="1:15" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="55"/>
-      <c r="B14" s="120">
-        <v>7006</v>
-      </c>
-      <c r="C14" s="32"/>
-      <c r="D14" s="60"/>
-      <c r="E14" s="47"/>
-      <c r="F14" s="45"/>
-      <c r="G14" s="45"/>
-      <c r="H14" s="45"/>
-      <c r="I14" s="45"/>
-      <c r="K14" s="120">
-        <v>7006</v>
-      </c>
-      <c r="L14" s="103" t="s">
-        <v>28</v>
-      </c>
-      <c r="M14" s="69"/>
-      <c r="N14" s="69"/>
-      <c r="O14" s="69"/>
-    </row>
-    <row r="15" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="55"/>
-      <c r="B15" s="121">
-        <v>7008</v>
-      </c>
-      <c r="C15" s="112"/>
-      <c r="D15" s="113"/>
-      <c r="E15" s="114"/>
-      <c r="I15" s="45"/>
-      <c r="K15" s="120">
-        <v>7008</v>
-      </c>
-      <c r="L15" s="103" t="s">
-        <v>29</v>
-      </c>
-      <c r="M15" s="69"/>
-      <c r="N15" s="69"/>
-      <c r="O15" s="69"/>
-    </row>
-    <row r="16" spans="1:15" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="56"/>
-      <c r="B16" s="115" t="s">
-        <v>11</v>
-      </c>
-      <c r="C16" s="116"/>
-      <c r="D16" s="117"/>
-      <c r="E16" s="118"/>
-      <c r="I16" s="45"/>
-      <c r="K16" s="107"/>
-      <c r="L16" s="107"/>
-      <c r="M16" s="107"/>
-      <c r="N16" s="107"/>
-      <c r="O16" s="107"/>
-    </row>
-    <row r="17" spans="1:15" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="122"/>
-      <c r="K17" s="26"/>
-      <c r="L17" s="123" t="s">
-        <v>35</v>
-      </c>
-      <c r="M17" s="64"/>
-      <c r="N17" s="64"/>
-      <c r="O17" s="64"/>
-    </row>
-    <row r="18" spans="1:15" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="57"/>
-      <c r="K18" s="26"/>
-      <c r="L18" s="41" t="s">
-        <v>4</v>
-      </c>
-      <c r="M18" s="25"/>
-      <c r="N18" s="25"/>
-      <c r="O18" s="25"/>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A22" s="28">
-        <v>0</v>
-      </c>
-      <c r="L22" s="29">
-        <v>0</v>
-      </c>
-      <c r="M22" s="37"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A23" s="28"/>
-      <c r="L23" s="38" t="s">
-        <v>7</v>
-      </c>
-      <c r="M23" s="37"/>
+      <c r="A23" s="25"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="10">
     <mergeCell ref="N2:O2"/>
     <mergeCell ref="N3:O3"/>
     <mergeCell ref="N4:O4"/>
@@ -2538,7 +2547,11 @@
     <mergeCell ref="D6:D11"/>
     <mergeCell ref="E6:E11"/>
     <mergeCell ref="N6:O6"/>
+    <mergeCell ref="K9:K10"/>
   </mergeCells>
+  <conditionalFormatting sqref="K9">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Ruta de archivo Repostes adaptable
</commit_message>
<xml_diff>
--- a/Reporte/ReportesSigre.xlsx
+++ b/Reporte/ReportesSigre.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\SigreWeb\sigreweb-main\SigreApiRest\Reporte\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\sigreweb-main\sigreweb-main\app\Reporte\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45383497-7D6F-46E6-93CD-74FBE695B4AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82ABCE75-5711-48E2-856D-BF16A2CB2826}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1335" yWindow="750" windowWidth="25695" windowHeight="14055" xr2:uid="{4481B342-BB1C-481E-A30A-ED1416DC2C19}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4481B342-BB1C-481E-A30A-ED1416DC2C19}"/>
   </bookViews>
   <sheets>
     <sheet name="BT" sheetId="1" r:id="rId1"/>
@@ -59,9 +59,6 @@
     <t>Total</t>
   </si>
   <si>
-    <t>Cantidad para el presupuesto</t>
-  </si>
-  <si>
     <t>COMPONENTE DE ALUMBRADO PUBLICO</t>
   </si>
   <si>
@@ -119,9 +116,6 @@
     <t>POSTE BT</t>
   </si>
   <si>
-    <t xml:space="preserve">SED: </t>
-  </si>
-  <si>
     <t>CÓDIGOS</t>
   </si>
   <si>
@@ -144,6 +138,12 @@
   </si>
   <si>
     <t>ORDEN N°:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALIMENTADOR / SED: </t>
+  </si>
+  <si>
+    <t>Cantidad Total</t>
   </si>
 </sst>
 </file>
@@ -1386,6 +1386,9 @@
     <xf numFmtId="0" fontId="17" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="1" fontId="3" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" shrinkToFit="1"/>
     </xf>
@@ -1474,9 +1477,6 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1828,11 +1828,10 @@
     <col min="1" max="1" width="1.7109375" hidden="1" customWidth="1"/>
     <col min="2" max="2" width="2.28515625" hidden="1" customWidth="1"/>
     <col min="3" max="3" width="2.85546875" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="1.5703125" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="2" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="1.28515625" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="2" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="1.7109375" hidden="1" customWidth="1"/>
+    <col min="4" max="5" width="3" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="1.7109375" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="1.140625" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="1.5703125" hidden="1" customWidth="1"/>
     <col min="9" max="9" width="2.28515625" hidden="1" customWidth="1"/>
     <col min="10" max="10" width="4.85546875" customWidth="1"/>
     <col min="11" max="11" width="8" bestFit="1" customWidth="1"/>
@@ -1847,20 +1846,20 @@
     <row r="2" spans="1:22" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K2" s="1"/>
       <c r="L2" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="M2" s="3"/>
-      <c r="N2" s="138" t="s">
-        <v>12</v>
-      </c>
-      <c r="O2" s="139"/>
+      <c r="N2" s="139" t="s">
+        <v>11</v>
+      </c>
+      <c r="O2" s="140"/>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="K3" s="4"/>
       <c r="L3" s="5"/>
       <c r="M3" s="6"/>
-      <c r="N3" s="142"/>
-      <c r="O3" s="143"/>
+      <c r="N3" s="143"/>
+      <c r="O3" s="144"/>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="K4" s="4"/>
@@ -1868,17 +1867,17 @@
       <c r="M4" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="N4" s="144"/>
-      <c r="O4" s="145"/>
+      <c r="N4" s="145"/>
+      <c r="O4" s="146"/>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="K5" s="4"/>
       <c r="L5" s="9"/>
       <c r="M5" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="N5" s="144"/>
-      <c r="O5" s="145"/>
+        <v>36</v>
+      </c>
+      <c r="N5" s="145"/>
+      <c r="O5" s="146"/>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="K6" s="4"/>
@@ -1886,37 +1885,37 @@
       <c r="M6" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="N6" s="140"/>
-      <c r="O6" s="141"/>
+      <c r="N6" s="141"/>
+      <c r="O6" s="142"/>
     </row>
     <row r="7" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K7" s="10"/>
       <c r="L7" s="11"/>
       <c r="M7" s="62" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="N7" s="9"/>
       <c r="O7" s="60"/>
     </row>
     <row r="8" spans="1:22" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="13"/>
-      <c r="B8" s="126" t="s">
+      <c r="B8" s="127" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="129" t="s">
+      <c r="C8" s="130" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="135" t="s">
+      <c r="D8" s="136" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="132" t="s">
-        <v>10</v>
+      <c r="E8" s="133" t="s">
+        <v>37</v>
       </c>
       <c r="G8" s="37"/>
       <c r="H8" s="37"/>
       <c r="K8" s="111"/>
       <c r="L8" s="109" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="M8" s="13"/>
       <c r="N8" s="123"/>
@@ -1924,15 +1923,15 @@
     </row>
     <row r="9" spans="1:22" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="14"/>
-      <c r="B9" s="127"/>
-      <c r="C9" s="130"/>
-      <c r="D9" s="136"/>
-      <c r="E9" s="133"/>
+      <c r="B9" s="128"/>
+      <c r="C9" s="131"/>
+      <c r="D9" s="137"/>
+      <c r="E9" s="134"/>
       <c r="G9" s="37"/>
       <c r="H9" s="37"/>
       <c r="K9" s="56"/>
       <c r="L9" s="91" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M9" s="120"/>
       <c r="N9" s="121"/>
@@ -1941,15 +1940,15 @@
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" s="15"/>
-      <c r="B10" s="127"/>
-      <c r="C10" s="130"/>
-      <c r="D10" s="136"/>
-      <c r="E10" s="133"/>
+      <c r="B10" s="128"/>
+      <c r="C10" s="131"/>
+      <c r="D10" s="137"/>
+      <c r="E10" s="134"/>
       <c r="G10" s="37"/>
       <c r="H10" s="37"/>
       <c r="K10" s="81"/>
       <c r="L10" s="61" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M10" s="75"/>
       <c r="N10" s="64"/>
@@ -1958,17 +1957,17 @@
     </row>
     <row r="11" spans="1:22" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="16"/>
-      <c r="B11" s="127"/>
-      <c r="C11" s="131"/>
-      <c r="D11" s="136"/>
-      <c r="E11" s="133"/>
+      <c r="B11" s="128"/>
+      <c r="C11" s="132"/>
+      <c r="D11" s="137"/>
+      <c r="E11" s="134"/>
       <c r="G11" s="37"/>
       <c r="H11" s="37"/>
       <c r="K11" s="84">
         <v>6002</v>
       </c>
       <c r="L11" s="54" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="M11" s="75"/>
       <c r="N11" s="64"/>
@@ -1977,19 +1976,19 @@
     </row>
     <row r="12" spans="1:22" ht="55.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="16"/>
-      <c r="B12" s="128"/>
+      <c r="B12" s="129"/>
       <c r="C12" s="44">
         <v>0</v>
       </c>
-      <c r="D12" s="137"/>
-      <c r="E12" s="134"/>
+      <c r="D12" s="138"/>
+      <c r="E12" s="135"/>
       <c r="G12" s="37"/>
       <c r="H12" s="37"/>
       <c r="K12" s="84">
         <v>6004</v>
       </c>
       <c r="L12" s="54" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M12" s="75"/>
       <c r="N12" s="64"/>
@@ -2010,7 +2009,7 @@
         <v>6006</v>
       </c>
       <c r="L13" s="54" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M13" s="75"/>
       <c r="N13" s="64"/>
@@ -2031,7 +2030,7 @@
         <v>6008</v>
       </c>
       <c r="L14" s="82" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M14" s="76"/>
       <c r="N14" s="65"/>
@@ -2050,7 +2049,7 @@
       <c r="H15" s="38"/>
       <c r="K15" s="55"/>
       <c r="L15" s="91" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="M15" s="77"/>
       <c r="N15" s="63"/>
@@ -2071,7 +2070,7 @@
         <v>6024</v>
       </c>
       <c r="L16" s="61" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="M16" s="75"/>
       <c r="N16" s="64"/>
@@ -2090,7 +2089,7 @@
       <c r="H17" s="38"/>
       <c r="K17" s="89"/>
       <c r="L17" s="61" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M17" s="78"/>
       <c r="N17" s="66"/>
@@ -2107,7 +2106,7 @@
       <c r="E18" s="40"/>
       <c r="K18" s="55"/>
       <c r="L18" s="91" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="M18" s="77"/>
       <c r="N18" s="63"/>
@@ -2128,7 +2127,7 @@
         <v>6026</v>
       </c>
       <c r="L19" s="61" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="M19" s="75"/>
       <c r="N19" s="64"/>
@@ -2148,7 +2147,7 @@
         <v>6028</v>
       </c>
       <c r="L20" s="94" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="M20" s="75"/>
       <c r="N20" s="64"/>
@@ -2168,7 +2167,7 @@
       </c>
       <c r="K22" s="93"/>
       <c r="L22" s="115" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="M22" s="112"/>
       <c r="N22" s="113"/>
@@ -2178,7 +2177,7 @@
       <c r="A23" s="20"/>
       <c r="K23" s="4"/>
       <c r="L23" s="106" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="M23" s="79"/>
       <c r="N23" s="67"/>
@@ -2248,7 +2247,7 @@
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="12" topLeftCell="M1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="N7" sqref="N7"/>
+      <selection pane="topRight" activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2257,11 +2256,11 @@
     <col min="2" max="2" width="2.7109375" hidden="1" customWidth="1"/>
     <col min="3" max="3" width="2.28515625" hidden="1" customWidth="1"/>
     <col min="4" max="4" width="3.5703125" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="6.42578125" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="6.85546875" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="5.7109375" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="5.85546875" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="4.140625" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="2.5703125" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="2.140625" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="2.5703125" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="1.42578125" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="2.140625" hidden="1" customWidth="1"/>
     <col min="10" max="10" width="4.85546875" customWidth="1"/>
     <col min="11" max="11" width="7.7109375" customWidth="1"/>
     <col min="12" max="12" width="80.140625" bestFit="1" customWidth="1"/>
@@ -2276,17 +2275,17 @@
         <v>5</v>
       </c>
       <c r="M2" s="3"/>
-      <c r="N2" s="146" t="s">
+      <c r="N2" s="147" t="s">
         <v>4</v>
       </c>
-      <c r="O2" s="147"/>
+      <c r="O2" s="148"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="K3" s="4"/>
       <c r="L3" s="5"/>
       <c r="M3" s="6"/>
-      <c r="N3" s="142"/>
-      <c r="O3" s="143"/>
+      <c r="N3" s="143"/>
+      <c r="O3" s="144"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="K4" s="4"/>
@@ -2294,30 +2293,30 @@
       <c r="M4" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="N4" s="144"/>
-      <c r="O4" s="145"/>
+      <c r="N4" s="145"/>
+      <c r="O4" s="146"/>
     </row>
     <row r="5" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K5" s="4"/>
       <c r="L5" s="9"/>
       <c r="M5" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="N5" s="144"/>
-      <c r="O5" s="145"/>
+        <v>36</v>
+      </c>
+      <c r="N5" s="145"/>
+      <c r="O5" s="146"/>
     </row>
     <row r="6" spans="1:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="148" t="s">
+      <c r="B6" s="149" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="151" t="s">
+      <c r="C6" s="152" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="154" t="s">
+      <c r="D6" s="155" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="156" t="s">
-        <v>10</v>
+      <c r="E6" s="157" t="s">
+        <v>37</v>
       </c>
       <c r="F6" s="37"/>
       <c r="G6" s="37"/>
@@ -2328,28 +2327,28 @@
       <c r="M6" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="N6" s="140"/>
-      <c r="O6" s="141"/>
+      <c r="N6" s="141"/>
+      <c r="O6" s="142"/>
     </row>
     <row r="7" spans="1:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="149"/>
-      <c r="C7" s="152"/>
-      <c r="D7" s="149"/>
-      <c r="E7" s="149"/>
+      <c r="B7" s="150"/>
+      <c r="C7" s="153"/>
+      <c r="D7" s="150"/>
+      <c r="E7" s="150"/>
       <c r="I7" s="37"/>
       <c r="K7" s="10"/>
       <c r="L7" s="11"/>
       <c r="M7" s="62" t="s">
-        <v>37</v>
-      </c>
-      <c r="N7" s="159"/>
+        <v>35</v>
+      </c>
+      <c r="N7" s="126"/>
       <c r="O7" s="12"/>
     </row>
     <row r="8" spans="1:15" ht="18.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="149"/>
-      <c r="C8" s="152"/>
-      <c r="D8" s="149"/>
-      <c r="E8" s="149"/>
+      <c r="B8" s="150"/>
+      <c r="C8" s="153"/>
+      <c r="D8" s="150"/>
+      <c r="E8" s="150"/>
       <c r="I8" s="37"/>
       <c r="K8" s="116"/>
       <c r="L8" s="110"/>
@@ -2359,16 +2358,16 @@
     </row>
     <row r="9" spans="1:15" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="45"/>
-      <c r="B9" s="149"/>
-      <c r="C9" s="152"/>
-      <c r="D9" s="149"/>
-      <c r="E9" s="149"/>
+      <c r="B9" s="150"/>
+      <c r="C9" s="153"/>
+      <c r="D9" s="150"/>
+      <c r="E9" s="150"/>
       <c r="I9" s="37"/>
-      <c r="K9" s="157" t="s">
-        <v>30</v>
+      <c r="K9" s="158" t="s">
+        <v>28</v>
       </c>
       <c r="L9" s="118" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="M9" s="21"/>
       <c r="N9" s="21"/>
@@ -2376,14 +2375,14 @@
     </row>
     <row r="10" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="46"/>
-      <c r="B10" s="149"/>
-      <c r="C10" s="153"/>
-      <c r="D10" s="149"/>
-      <c r="E10" s="149"/>
+      <c r="B10" s="150"/>
+      <c r="C10" s="154"/>
+      <c r="D10" s="150"/>
+      <c r="E10" s="150"/>
       <c r="I10" s="37"/>
-      <c r="K10" s="158"/>
+      <c r="K10" s="159"/>
       <c r="L10" s="117" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="M10" s="22"/>
       <c r="N10" s="22"/>
@@ -2391,16 +2390,16 @@
     </row>
     <row r="11" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="47"/>
-      <c r="B11" s="150"/>
+      <c r="B11" s="151"/>
       <c r="C11" s="51">
         <v>0</v>
       </c>
-      <c r="D11" s="155"/>
-      <c r="E11" s="155"/>
+      <c r="D11" s="156"/>
+      <c r="E11" s="156"/>
       <c r="I11" s="37"/>
       <c r="K11" s="91"/>
       <c r="L11" s="91" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="M11" s="91"/>
       <c r="N11" s="91"/>
@@ -2422,7 +2421,7 @@
         <v>7002</v>
       </c>
       <c r="L12" s="58" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M12" s="23"/>
       <c r="N12" s="23"/>
@@ -2444,7 +2443,7 @@
         <v>7004</v>
       </c>
       <c r="L13" s="87" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="M13" s="108"/>
       <c r="N13" s="108"/>
@@ -2466,7 +2465,7 @@
         <v>7006</v>
       </c>
       <c r="L14" s="88" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="M14" s="59"/>
       <c r="N14" s="59"/>
@@ -2485,7 +2484,7 @@
         <v>7008</v>
       </c>
       <c r="L15" s="88" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="M15" s="59"/>
       <c r="N15" s="59"/>
@@ -2502,7 +2501,7 @@
       <c r="I16" s="38"/>
       <c r="K16" s="91"/>
       <c r="L16" s="119" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="M16" s="125"/>
       <c r="N16" s="125"/>
@@ -2512,7 +2511,7 @@
       <c r="A17" s="105"/>
       <c r="K17" s="23"/>
       <c r="L17" s="106" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="M17" s="57"/>
       <c r="N17" s="57"/>

</xml_diff>